<commit_message>
Update .ino y testing
</commit_message>
<xml_diff>
--- a/06 Revisiones y Testing/Testing.xlsx
+++ b/06 Revisiones y Testing/Testing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Prueba</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>1 Las presiones de operación normales ( sin paciente en la mascara) no rebasaron los 20 cmH2O</t>
+  </si>
+  <si>
+    <t>Motor salta a 40cmH2O</t>
   </si>
 </sst>
 </file>
@@ -490,11 +493,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="229178184"/>
-        <c:axId val="229177008"/>
+        <c:axId val="217875984"/>
+        <c:axId val="217876376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="229178184"/>
+        <c:axId val="217875984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -607,12 +610,12 @@
             <a:endParaRPr lang="es-NI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229177008"/>
+        <c:crossAx val="217876376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="229177008"/>
+        <c:axId val="217876376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -725,7 +728,7 @@
             <a:endParaRPr lang="es-NI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229178184"/>
+        <c:crossAx val="217875984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1660,10 +1663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H35"/>
+  <dimension ref="A2:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2000,6 +2003,11 @@
         <v>30</v>
       </c>
     </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>